<commit_message>
Finalized Week 5 doc.
</commit_message>
<xml_diff>
--- a/Wk 5 Submission/Equiv table.xlsx
+++ b/Wk 5 Submission/Equiv table.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="18">
   <si>
     <t>Side 1</t>
   </si>
@@ -61,13 +61,22 @@
   </si>
   <si>
     <t>Non-Numeric Character</t>
+  </si>
+  <si>
+    <t>Isoceles</t>
+  </si>
+  <si>
+    <t>Right Angle Percision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,8 +96,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,8 +117,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -114,30 +136,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -184,20 +182,15 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -213,9 +206,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -225,44 +216,42 @@
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,15 +554,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" style="1" customWidth="1"/>
     <col min="3" max="4" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
@@ -584,343 +573,417 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="8"/>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="7"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="10">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10">
         <v>3</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="10">
         <v>4</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="10">
         <v>5</v>
       </c>
-      <c r="G2" s="2">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2">
-        <v>7</v>
-      </c>
-      <c r="I2" s="3">
+      <c r="G2" s="10">
+        <v>6</v>
+      </c>
+      <c r="H2" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.41</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="F6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="14"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="10">
+        <v>8</v>
+      </c>
+      <c r="C11" s="10">
+        <v>9</v>
+      </c>
+      <c r="D11" s="10">
+        <v>10</v>
+      </c>
+      <c r="E11" s="10">
+        <v>11</v>
+      </c>
+      <c r="F11" s="10">
+        <v>12</v>
+      </c>
+      <c r="G11" s="10">
+        <v>13</v>
+      </c>
+      <c r="H11" s="10">
+        <v>14</v>
+      </c>
+      <c r="I11" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="12">
-        <v>1</v>
-      </c>
-      <c r="D3" s="12">
-        <v>1</v>
-      </c>
-      <c r="E3" s="12">
-        <v>1</v>
-      </c>
-      <c r="F3" s="12">
-        <v>1</v>
-      </c>
-      <c r="G3" s="12">
-        <v>1</v>
-      </c>
-      <c r="H3" s="12">
+      <c r="B12" s="2">
         <v>3</v>
       </c>
-      <c r="I3" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="12">
-        <v>1</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="12">
-        <v>2</v>
-      </c>
-      <c r="E4" s="12">
-        <v>1</v>
-      </c>
-      <c r="F4" s="12">
-        <v>2</v>
-      </c>
-      <c r="G4" s="12">
-        <v>1</v>
-      </c>
-      <c r="H4" s="12">
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>10</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2">
         <v>4</v>
       </c>
-      <c r="I4" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="12">
-        <v>2</v>
-      </c>
-      <c r="C5" s="12">
-        <v>2</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="12">
-        <v>1</v>
-      </c>
-      <c r="F5" s="12">
-        <v>2</v>
-      </c>
-      <c r="G5" s="12">
-        <v>1.41</v>
-      </c>
-      <c r="H5" s="12">
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2</v>
+      </c>
+      <c r="I13" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2">
         <v>5</v>
       </c>
-      <c r="I5" s="12">
+      <c r="C14" s="2">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="D14" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="13" t="s">
+      <c r="E14" s="2">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="2">
+        <v>10</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="C15" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="12" t="s">
+      <c r="B16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="2">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2">
-        <v>11</v>
-      </c>
-      <c r="E11" s="2">
-        <v>12</v>
-      </c>
-      <c r="F11" s="2">
-        <v>13</v>
-      </c>
-      <c r="G11" s="3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="63" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="12">
-        <v>10</v>
-      </c>
-      <c r="G12" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="12">
-        <v>2</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="12">
-        <v>2</v>
-      </c>
-      <c r="E13" s="12">
-        <v>2</v>
-      </c>
-      <c r="F13" s="12">
-        <v>2</v>
-      </c>
-      <c r="G13" s="12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="12">
-        <v>3</v>
-      </c>
-      <c r="C14" s="12">
-        <v>3</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="12">
-        <v>10</v>
-      </c>
-      <c r="F14" s="12">
-        <v>1</v>
-      </c>
-      <c r="G14" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>6</v>
+      <c r="C16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B1:I1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>